<commit_message>
adds links to files github database
</commit_message>
<xml_diff>
--- a/PDE3 database - Institute of Translational Medicine - University of Liverpool.xlsx
+++ b/PDE3 database - Institute of Translational Medicine - University of Liverpool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivbie\Documents\2020 - Projetos mestrado\CYFIP2\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAE0891-B3D2-4D4A-9110-BD4FD1CD1D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C12425-A7E0-42C5-AA8D-3C9F66A05400}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1504,7 +1504,7 @@
     <t>Compound Name</t>
   </si>
   <si>
-    <t>https://1drv.ms/u/s!AhSq1zsYbWoogbRnTraaotSvfFzNdg?e=hkNSgd</t>
+    <t>https://github.com/isisventbiem/pde3database</t>
   </si>
 </sst>
 </file>
@@ -8202,7 +8202,7 @@
   <dimension ref="B2:F175"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
adds new files to database
</commit_message>
<xml_diff>
--- a/PDE3 database - Institute of Translational Medicine - University of Liverpool.xlsx
+++ b/PDE3 database - Institute of Translational Medicine - University of Liverpool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivbie\Documents\2020 - Projetos mestrado\CYFIP2\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28138C4-CD3E-4400-B5D0-C4811DA48218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5281B1B-0128-4949-82DA-8FA3A0B77E87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="658">
   <si>
     <t>Name</t>
   </si>
@@ -973,9 +973,6 @@
     <t>Levobupivacaine</t>
   </si>
   <si>
-    <t>Thalidomide</t>
-  </si>
-  <si>
     <t>Malignant disease; immunosuppression</t>
   </si>
   <si>
@@ -1634,6 +1631,378 @@
   </si>
   <si>
     <t>https://github.com/isisventbiem/pde3database/blob/master/PDB%20files%20from%20HIC-Up/Formula%20C9%20H8%20O4.txt</t>
+  </si>
+  <si>
+    <t>C20 H25 Cl N2 O5</t>
+  </si>
+  <si>
+    <t>C4 H11 N5</t>
+  </si>
+  <si>
+    <t>C20 H21 F N2 O</t>
+  </si>
+  <si>
+    <t>C20 H23 N</t>
+  </si>
+  <si>
+    <t>C17 H17 Cl2 N</t>
+  </si>
+  <si>
+    <t>C22 H23 Cl N6 O</t>
+  </si>
+  <si>
+    <t>C14 H14 O3</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_33741</t>
+  </si>
+  <si>
+    <t>SC17 H18 F3 N O</t>
+  </si>
+  <si>
+    <t>RC17 H18 F3 N O</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5656</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_9782</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5002</t>
+  </si>
+  <si>
+    <t>C20 H24 N2 O2</t>
+  </si>
+  <si>
+    <t>C22 H26 N2 O4 S</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_54687</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4095</t>
+  </si>
+  <si>
+    <t>C17 H18 N2 O6</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5388962</t>
+  </si>
+  <si>
+    <t>C18 H19 N O S</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5073</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_2471</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_2725</t>
+  </si>
+  <si>
+    <t>C14 H22 N2 O</t>
+  </si>
+  <si>
+    <t>C22 H28 N2 O</t>
+  </si>
+  <si>
+    <t>C10 H12 Cl N O2</t>
+  </si>
+  <si>
+    <t>C12 H21 N</t>
+  </si>
+  <si>
+    <t>C19 H20 N2 O3 S</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_6279</t>
+  </si>
+  <si>
+    <t>C23 H27 Cl2 N3 O2</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4168</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4927</t>
+  </si>
+  <si>
+    <t>C27 H38 N2 O4</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5732</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4171</t>
+  </si>
+  <si>
+    <t>C22 H29 F O5</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3658</t>
+  </si>
+  <si>
+    <t>C25 H29 I2 N O3</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3108</t>
+  </si>
+  <si>
+    <t>C9 H9 Cl2 N3</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_132999</t>
+  </si>
+  <si>
+    <t>C33 H30 N4 O2</t>
+  </si>
+  <si>
+    <t>C21 H23 Cl F N O2</t>
+  </si>
+  <si>
+    <t>C17 H19 Cl N2 S</t>
+  </si>
+  <si>
+    <t>C15 H15 N O2</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_1548943</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_56959</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4595</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_2477</t>
+  </si>
+  <si>
+    <t>C19 H24 N2</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5572</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5487</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4236</t>
+  </si>
+  <si>
+    <t>C19 H21 N5 O4</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3117</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_6914273</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_26757</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_667477</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4601</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4474</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_2955</t>
+  </si>
+  <si>
+    <t>C15 H21 F3 N2 O2</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4932</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_444</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_2200</t>
+  </si>
+  <si>
+    <t>C8 H5 F3 N2 O S</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_2474</t>
+  </si>
+  <si>
+    <t>C15 H24 N2 O2</t>
+  </si>
+  <si>
+    <t>C32 H40 Br N5 O5</t>
+  </si>
+  <si>
+    <t>C17 H16 F6 N2 O</t>
+  </si>
+  <si>
+    <t>C17 H17 N O2</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5282381</t>
+  </si>
+  <si>
+    <t>C12 H11 N7</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4828</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_135398737</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_16362</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3516</t>
+  </si>
+  <si>
+    <t>C8 H7 Cl N2 O2 S</t>
+  </si>
+  <si>
+    <t>C21 H21 N</t>
+  </si>
+  <si>
+    <t>C19 H27 N O</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4064</t>
+  </si>
+  <si>
+    <t>C18 H18 N8 O7 S3</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5593</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3784</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_47811</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4911</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4768</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3397</t>
+  </si>
+  <si>
+    <t>C21 H26 N2 O7</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5360696</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_6041</t>
+  </si>
+  <si>
+    <t>C21 H26 N2 S2</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_92253</t>
+  </si>
+  <si>
+    <t>S-Thalidomide</t>
+  </si>
+  <si>
+    <t>C13 H10 N2 O4</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4636</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_2381</t>
+  </si>
+  <si>
+    <t>C22 H32 O4</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_6047</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4499</t>
+  </si>
+  <si>
+    <t>C13 H16 N2 O2</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_6729</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5361092</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5311068</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3042</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3226</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5870</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3487</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5702063</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4032</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4058</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_10836</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_6082</t>
+  </si>
+  <si>
+    <t>C21 H27 N3 O2</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4688</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4761</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5775</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5794</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_4914</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_638678</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_208902</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_5770</t>
+  </si>
+  <si>
+    <t>C17 H14 O4 S</t>
+  </si>
+  <si>
+    <t>Conformer3D_CID_3000322</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +2085,27 @@
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1946,17 +2335,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B424DCE3-2D94-4B01-8D4C-13D38CF07CAE}" name="Tabela1" displayName="Tabela1" ref="B2:Q174" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B424DCE3-2D94-4B01-8D4C-13D38CF07CAE}" name="Tabela1" displayName="Tabela1" ref="B2:Q174" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="B2:Q174" xr:uid="{4AB5E234-523A-40D6-A65E-0BBB1D90474A}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{4D3698C4-EA49-4C98-83ED-B651DA65BAD9}" name="Compound ID" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{4D3698C4-EA49-4C98-83ED-B651DA65BAD9}" name="Compound ID" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{1A309358-CA89-41E0-9A90-F70309D9DB35}" name="Name"/>
     <tableColumn id="3" xr3:uid="{D13F5563-5245-4C67-94CA-3D8EDEFE37DF}" name="Indications"/>
-    <tableColumn id="4" xr3:uid="{76964F19-9FCA-42C4-B5B4-2AF969873583}" name="First licensed (year)" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{B915C42A-C3AD-4EE8-B307-583A94B2DF61}" name="Prescriptions items dispensed in England in 2016 (number)" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{1B0C2226-493B-4FBE-99AD-673CA85A1B15}" name="Prescriptions items dispensed in England in 2016 (rank)" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{D6EC2CBC-8C62-4043-BB6D-10AA76365A08}" name="Number of studies" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{0A534E60-C891-4915-8B75-E57E2E5FF298}" name="Number of unique models" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{76964F19-9FCA-42C4-B5B4-2AF969873583}" name="First licensed (year)" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{B915C42A-C3AD-4EE8-B307-583A94B2DF61}" name="Prescriptions items dispensed in England in 2016 (number)" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{1B0C2226-493B-4FBE-99AD-673CA85A1B15}" name="Prescriptions items dispensed in England in 2016 (rank)" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{D6EC2CBC-8C62-4043-BB6D-10AA76365A08}" name="Number of studies" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{0A534E60-C891-4915-8B75-E57E2E5FF298}" name="Number of unique models" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{A9116F38-0E87-4451-8ABE-9A3C77A0A932}" name="Models"/>
     <tableColumn id="10" xr3:uid="{29B8A375-527D-4674-B623-E53F6154EE54}" name="AEDs enhanced"/>
     <tableColumn id="11" xr3:uid="{1CDE8E53-BAB9-4B1F-B65F-C4873C03DFE7}" name="Number of studies2"/>
@@ -1971,14 +2360,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54767107-61A5-4E5F-84FA-2A8D9B5C4D10}" name="Tabela2" displayName="Tabela2" ref="B2:F175" totalsRowCount="1" headerRowDxfId="6">
-  <autoFilter ref="B2:F174" xr:uid="{2A0284F6-0E4E-4CE1-9526-7ACFD806AE5D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54767107-61A5-4E5F-84FA-2A8D9B5C4D10}" name="Tabela2" displayName="Tabela2" ref="B2:F176" totalsRowCount="1" headerRowDxfId="8">
+  <autoFilter ref="B2:F175" xr:uid="{2A0284F6-0E4E-4CE1-9526-7ACFD806AE5D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F07FB46E-2261-4395-95B4-499CFE4DC5CC}" name="File ID" totalsRowLabel="Total" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{824CA5B7-C3F1-4EF2-BF5E-B7E729203F26}" name="Compound ID" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{F07FB46E-2261-4395-95B4-499CFE4DC5CC}" name="File ID" totalsRowLabel="Total" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{824CA5B7-C3F1-4EF2-BF5E-B7E729203F26}" name="Compound ID" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{8E5ABDBD-3B43-49EC-BA36-F6AADA0EA1ED}" name="Compound Name"/>
     <tableColumn id="3" xr3:uid="{18BA9869-4705-4B91-9295-CA0136FABA04}" name="File Name" totalsRowFunction="count"/>
-    <tableColumn id="4" xr3:uid="{FB23DE31-DBC1-42B4-ABAA-CDF6F245AAEB}" name="File Adress" totalsRowFunction="count" dataDxfId="3" dataCellStyle="Hiperlink"/>
+    <tableColumn id="4" xr3:uid="{FB23DE31-DBC1-42B4-ABAA-CDF6F245AAEB}" name="File Adress" totalsRowFunction="count" dataDxfId="5" dataCellStyle="Hiperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2283,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R178"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" topLeftCell="A139" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D162" sqref="D162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -2312,7 +2701,7 @@
     <row r="1" spans="2:17"/>
     <row r="2" spans="2:17">
       <c r="B2" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -2342,22 +2731,22 @@
         <v>8</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="3" spans="2:17">
@@ -2401,10 +2790,10 @@
         <v>1</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Q3" t="s">
         <v>13</v>
@@ -2451,7 +2840,7 @@
         <v>1</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" t="s">
@@ -2499,7 +2888,7 @@
         <v>1</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" t="s">
@@ -2626,7 +3015,7 @@
         <v>1</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="P8" s="4"/>
     </row>
@@ -2671,7 +3060,7 @@
         <v>0</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" t="s">
@@ -2798,7 +3187,7 @@
         <v>0</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="P12" s="4"/>
     </row>
@@ -2843,7 +3232,7 @@
         <v>1</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" t="s">
@@ -2911,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P15" s="4"/>
     </row>
@@ -2985,7 +3374,7 @@
         <v>1</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" t="s">
@@ -3106,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Q20" t="s">
         <v>26</v>
@@ -3188,7 +3577,7 @@
         <v>1</v>
       </c>
       <c r="O22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="23" spans="2:17">
@@ -3281,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="O25" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="26" spans="2:17">
@@ -3398,7 +3787,7 @@
         <v>0</v>
       </c>
       <c r="O28" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="Q28" t="s">
         <v>90</v>
@@ -3436,7 +3825,7 @@
         <v>1</v>
       </c>
       <c r="O29" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="30" spans="2:17">
@@ -3471,7 +3860,7 @@
         <v>1</v>
       </c>
       <c r="O30" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="31" spans="2:17">
@@ -3535,7 +3924,7 @@
         <v>1</v>
       </c>
       <c r="O32" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="33" spans="2:17">
@@ -3681,7 +4070,7 @@
         <v>1</v>
       </c>
       <c r="O36" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P36" s="3"/>
       <c r="Q36" t="s">
@@ -3749,7 +4138,7 @@
         <v>1</v>
       </c>
       <c r="O38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="39" spans="2:17">
@@ -3828,7 +4217,7 @@
         <v>1</v>
       </c>
       <c r="O40" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="41" spans="2:17">
@@ -3863,7 +4252,7 @@
         <v>1</v>
       </c>
       <c r="O41" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="42" spans="2:17">
@@ -3898,7 +4287,7 @@
         <v>1</v>
       </c>
       <c r="O42" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="43" spans="2:17">
@@ -3933,7 +4322,7 @@
         <v>1</v>
       </c>
       <c r="O43" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="44" spans="2:17">
@@ -4114,7 +4503,7 @@
         <v>1</v>
       </c>
       <c r="O48" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="49" spans="2:17">
@@ -4280,7 +4669,7 @@
         <v>0</v>
       </c>
       <c r="O53" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="54" spans="2:17">
@@ -4324,7 +4713,7 @@
         <v>0</v>
       </c>
       <c r="O54" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P54" s="3"/>
       <c r="Q54" t="s">
@@ -4372,7 +4761,7 @@
         <v>1</v>
       </c>
       <c r="O55" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="P55" s="3"/>
       <c r="Q55" t="s">
@@ -4527,7 +4916,7 @@
         <v>1</v>
       </c>
       <c r="O60" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="61" spans="2:17">
@@ -4562,7 +4951,7 @@
         <v>1</v>
       </c>
       <c r="O61" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="62" spans="2:17">
@@ -4670,7 +5059,7 @@
         <v>1</v>
       </c>
       <c r="O64" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="65" spans="2:17">
@@ -4792,7 +5181,7 @@
         <v>1</v>
       </c>
       <c r="O68" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="69" spans="2:17">
@@ -4897,7 +5286,7 @@
         <v>1</v>
       </c>
       <c r="O71" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="P71" s="3"/>
       <c r="Q71" t="s">
@@ -5009,7 +5398,7 @@
         <v>0</v>
       </c>
       <c r="O74" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="P74" s="6"/>
     </row>
@@ -5089,7 +5478,7 @@
         <v>1</v>
       </c>
       <c r="O76" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="77" spans="2:17">
@@ -5252,7 +5641,7 @@
         <v>0</v>
       </c>
       <c r="O80" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="P80" s="3"/>
       <c r="Q80" t="s">
@@ -5453,7 +5842,7 @@
         <v>1</v>
       </c>
       <c r="O86" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="87" spans="2:17">
@@ -5532,7 +5921,7 @@
         <v>0</v>
       </c>
       <c r="O88" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="89" spans="2:17">
@@ -5713,7 +6102,7 @@
         <v>1</v>
       </c>
       <c r="O93" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="94" spans="2:17">
@@ -5792,7 +6181,7 @@
         <v>1</v>
       </c>
       <c r="O95" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="96" spans="2:17">
@@ -6118,7 +6507,7 @@
         <v>0</v>
       </c>
       <c r="O105" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="106" spans="2:17">
@@ -6153,7 +6542,7 @@
         <v>1</v>
       </c>
       <c r="O106" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="107" spans="2:17">
@@ -6377,7 +6766,7 @@
         <v>1</v>
       </c>
       <c r="O113" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="114" spans="2:17">
@@ -6746,7 +7135,7 @@
         <v>1</v>
       </c>
       <c r="O125" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="126" spans="2:17">
@@ -6863,7 +7252,7 @@
         <v>1</v>
       </c>
       <c r="O128" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="P128" s="3"/>
       <c r="Q128" t="s">
@@ -6902,7 +7291,7 @@
         <v>1</v>
       </c>
       <c r="O129" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="130" spans="2:17">
@@ -6968,10 +7357,10 @@
         <v>130</v>
       </c>
       <c r="C132" t="s">
+        <v>627</v>
+      </c>
+      <c r="D132" t="s">
         <v>314</v>
-      </c>
-      <c r="D132" t="s">
-        <v>315</v>
       </c>
       <c r="E132" s="3">
         <v>1998</v>
@@ -6997,7 +7386,7 @@
         <v>131</v>
       </c>
       <c r="C133" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D133" t="s">
         <v>55</v>
@@ -7026,10 +7415,10 @@
         <v>132</v>
       </c>
       <c r="C134" t="s">
+        <v>316</v>
+      </c>
+      <c r="D134" t="s">
         <v>317</v>
-      </c>
-      <c r="D134" t="s">
-        <v>318</v>
       </c>
       <c r="E134" s="3">
         <v>1986</v>
@@ -7055,10 +7444,10 @@
         <v>133</v>
       </c>
       <c r="C135" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="D135" t="s">
         <v>319</v>
-      </c>
-      <c r="D135" t="s">
-        <v>320</v>
       </c>
       <c r="E135" s="3">
         <v>1980</v>
@@ -7084,7 +7473,7 @@
         <v>134</v>
       </c>
       <c r="C136" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D136" t="s">
         <v>230</v>
@@ -7113,10 +7502,10 @@
         <v>135</v>
       </c>
       <c r="C137" t="s">
+        <v>321</v>
+      </c>
+      <c r="D137" t="s">
         <v>322</v>
-      </c>
-      <c r="D137" t="s">
-        <v>323</v>
       </c>
       <c r="E137" s="3">
         <v>2004</v>
@@ -7142,7 +7531,7 @@
         <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D138" t="s">
         <v>230</v>
@@ -7171,7 +7560,7 @@
         <v>137</v>
       </c>
       <c r="C139" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D139" t="s">
         <v>173</v>
@@ -7200,10 +7589,10 @@
         <v>138</v>
       </c>
       <c r="C140" t="s">
+        <v>325</v>
+      </c>
+      <c r="D140" t="s">
         <v>326</v>
-      </c>
-      <c r="D140" t="s">
-        <v>327</v>
       </c>
       <c r="E140" s="3">
         <v>1980</v>
@@ -7221,10 +7610,10 @@
         <v>2</v>
       </c>
       <c r="J140" t="s">
+        <v>327</v>
+      </c>
+      <c r="K140" t="s">
         <v>328</v>
-      </c>
-      <c r="K140" t="s">
-        <v>329</v>
       </c>
       <c r="L140" s="3">
         <v>2</v>
@@ -7244,10 +7633,10 @@
         <v>139</v>
       </c>
       <c r="C141" t="s">
+        <v>329</v>
+      </c>
+      <c r="D141" t="s">
         <v>330</v>
-      </c>
-      <c r="D141" t="s">
-        <v>331</v>
       </c>
       <c r="E141" s="3">
         <v>1982</v>
@@ -7273,10 +7662,10 @@
         <v>140</v>
       </c>
       <c r="C142" t="s">
+        <v>331</v>
+      </c>
+      <c r="D142" t="s">
         <v>332</v>
-      </c>
-      <c r="D142" t="s">
-        <v>333</v>
       </c>
       <c r="E142" s="3">
         <v>1978</v>
@@ -7317,10 +7706,10 @@
         <v>141</v>
       </c>
       <c r="C143" t="s">
+        <v>333</v>
+      </c>
+      <c r="D143" t="s">
         <v>334</v>
-      </c>
-      <c r="D143" t="s">
-        <v>335</v>
       </c>
       <c r="E143" s="3">
         <v>1982</v>
@@ -7346,10 +7735,10 @@
         <v>142</v>
       </c>
       <c r="C144" t="s">
+        <v>335</v>
+      </c>
+      <c r="D144" t="s">
         <v>336</v>
-      </c>
-      <c r="D144" t="s">
-        <v>337</v>
       </c>
       <c r="E144" s="3">
         <v>1994</v>
@@ -7367,7 +7756,7 @@
         <v>2</v>
       </c>
       <c r="J144" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="145" spans="2:17">
@@ -7375,10 +7764,10 @@
         <v>143</v>
       </c>
       <c r="C145" t="s">
+        <v>337</v>
+      </c>
+      <c r="D145" t="s">
         <v>338</v>
-      </c>
-      <c r="D145" t="s">
-        <v>339</v>
       </c>
       <c r="E145" s="3">
         <v>1964</v>
@@ -7419,10 +7808,10 @@
         <v>144</v>
       </c>
       <c r="C146" t="s">
+        <v>339</v>
+      </c>
+      <c r="D146" t="s">
         <v>340</v>
-      </c>
-      <c r="D146" t="s">
-        <v>341</v>
       </c>
       <c r="E146" s="3">
         <v>1999</v>
@@ -7440,7 +7829,7 @@
         <v>2</v>
       </c>
       <c r="J146" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="147" spans="2:17">
@@ -7448,10 +7837,10 @@
         <v>145</v>
       </c>
       <c r="C147" t="s">
+        <v>342</v>
+      </c>
+      <c r="D147" t="s">
         <v>343</v>
-      </c>
-      <c r="D147" t="s">
-        <v>344</v>
       </c>
       <c r="E147" s="3">
         <v>1950</v>
@@ -7477,7 +7866,7 @@
         <v>146</v>
       </c>
       <c r="C148" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D148" t="s">
         <v>258</v>
@@ -7506,10 +7895,10 @@
         <v>147</v>
       </c>
       <c r="C149" t="s">
+        <v>345</v>
+      </c>
+      <c r="D149" t="s">
         <v>346</v>
-      </c>
-      <c r="D149" t="s">
-        <v>347</v>
       </c>
       <c r="E149" s="3">
         <v>1979</v>
@@ -7535,7 +7924,7 @@
         <v>148</v>
       </c>
       <c r="C150" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D150" t="s">
         <v>151</v>
@@ -7564,7 +7953,7 @@
         <v>149</v>
       </c>
       <c r="C151" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D151" t="s">
         <v>173</v>
@@ -7593,7 +7982,7 @@
         <v>150</v>
       </c>
       <c r="C152" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D152" t="s">
         <v>258</v>
@@ -7622,7 +8011,7 @@
         <v>151</v>
       </c>
       <c r="C153" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D153" t="s">
         <v>258</v>
@@ -7651,7 +8040,7 @@
         <v>152</v>
       </c>
       <c r="C154" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D154" t="s">
         <v>290</v>
@@ -7680,7 +8069,7 @@
         <v>153</v>
       </c>
       <c r="C155" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D155" t="s">
         <v>10</v>
@@ -7701,7 +8090,7 @@
         <v>2</v>
       </c>
       <c r="J155" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K155" t="s">
         <v>12</v>
@@ -7716,7 +8105,7 @@
         <v>1</v>
       </c>
       <c r="O155" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="P155" s="3"/>
       <c r="Q155" t="s">
@@ -7728,10 +8117,10 @@
         <v>154</v>
       </c>
       <c r="C156" t="s">
+        <v>354</v>
+      </c>
+      <c r="D156" t="s">
         <v>355</v>
-      </c>
-      <c r="D156" t="s">
-        <v>356</v>
       </c>
       <c r="E156" s="3">
         <v>1956</v>
@@ -7757,10 +8146,10 @@
         <v>155</v>
       </c>
       <c r="C157" t="s">
+        <v>356</v>
+      </c>
+      <c r="D157" t="s">
         <v>357</v>
-      </c>
-      <c r="D157" t="s">
-        <v>358</v>
       </c>
       <c r="E157" s="3">
         <v>1980</v>
@@ -7786,7 +8175,7 @@
         <v>156</v>
       </c>
       <c r="C158" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D158" t="s">
         <v>55</v>
@@ -7815,10 +8204,10 @@
         <v>157</v>
       </c>
       <c r="C159" t="s">
+        <v>359</v>
+      </c>
+      <c r="D159" t="s">
         <v>360</v>
-      </c>
-      <c r="D159" t="s">
-        <v>361</v>
       </c>
       <c r="E159" s="3">
         <v>1943</v>
@@ -7859,10 +8248,10 @@
         <v>158</v>
       </c>
       <c r="C160" t="s">
+        <v>361</v>
+      </c>
+      <c r="D160" t="s">
         <v>362</v>
-      </c>
-      <c r="D160" t="s">
-        <v>363</v>
       </c>
       <c r="E160" s="3">
         <v>1982</v>
@@ -7888,10 +8277,10 @@
         <v>159</v>
       </c>
       <c r="C161" t="s">
+        <v>363</v>
+      </c>
+      <c r="D161" t="s">
         <v>364</v>
-      </c>
-      <c r="D161" t="s">
-        <v>365</v>
       </c>
       <c r="E161" s="3">
         <v>1962</v>
@@ -7917,7 +8306,7 @@
         <v>160</v>
       </c>
       <c r="C162" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D162" t="s">
         <v>108</v>
@@ -7953,7 +8342,7 @@
         <v>1</v>
       </c>
       <c r="O162" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="P162" s="3"/>
       <c r="Q162" t="s">
@@ -7965,10 +8354,10 @@
         <v>161</v>
       </c>
       <c r="C163" t="s">
+        <v>366</v>
+      </c>
+      <c r="D163" t="s">
         <v>367</v>
-      </c>
-      <c r="D163" t="s">
-        <v>368</v>
       </c>
       <c r="E163" s="3">
         <v>1982</v>
@@ -7994,10 +8383,10 @@
         <v>162</v>
       </c>
       <c r="C164" t="s">
+        <v>368</v>
+      </c>
+      <c r="D164" t="s">
         <v>369</v>
-      </c>
-      <c r="D164" t="s">
-        <v>370</v>
       </c>
       <c r="E164" s="3">
         <v>1994</v>
@@ -8023,7 +8412,7 @@
         <v>163</v>
       </c>
       <c r="C165" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D165" t="s">
         <v>300</v>
@@ -8052,10 +8441,10 @@
         <v>164</v>
       </c>
       <c r="C166" t="s">
+        <v>371</v>
+      </c>
+      <c r="D166" t="s">
         <v>372</v>
-      </c>
-      <c r="D166" t="s">
-        <v>373</v>
       </c>
       <c r="E166" s="3">
         <v>2000</v>
@@ -8081,7 +8470,7 @@
         <v>165</v>
       </c>
       <c r="C167" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D167" t="s">
         <v>258</v>
@@ -8102,7 +8491,7 @@
         <v>2</v>
       </c>
       <c r="J167" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K167" t="s">
         <v>41</v>
@@ -8125,10 +8514,10 @@
         <v>166</v>
       </c>
       <c r="C168" t="s">
+        <v>375</v>
+      </c>
+      <c r="D168" t="s">
         <v>376</v>
-      </c>
-      <c r="D168" t="s">
-        <v>377</v>
       </c>
       <c r="E168" s="3">
         <v>1976</v>
@@ -8154,7 +8543,7 @@
         <v>167</v>
       </c>
       <c r="C169" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D169" t="s">
         <v>151</v>
@@ -8183,10 +8572,10 @@
         <v>168</v>
       </c>
       <c r="C170" t="s">
+        <v>378</v>
+      </c>
+      <c r="D170" t="s">
         <v>379</v>
-      </c>
-      <c r="D170" t="s">
-        <v>380</v>
       </c>
       <c r="E170" s="3">
         <v>1960</v>
@@ -8212,10 +8601,10 @@
         <v>169</v>
       </c>
       <c r="C171" t="s">
+        <v>380</v>
+      </c>
+      <c r="D171" t="s">
         <v>381</v>
-      </c>
-      <c r="D171" t="s">
-        <v>382</v>
       </c>
       <c r="E171" s="3">
         <v>1999</v>
@@ -8233,10 +8622,10 @@
         <v>2</v>
       </c>
       <c r="J171" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K171" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L171" s="3">
         <v>2</v>
@@ -8248,7 +8637,7 @@
         <v>0</v>
       </c>
       <c r="O171" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="P171" s="3"/>
       <c r="Q171" t="s">
@@ -8260,7 +8649,7 @@
         <v>170</v>
       </c>
       <c r="C172" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D172" t="s">
         <v>173</v>
@@ -8289,10 +8678,10 @@
         <v>171</v>
       </c>
       <c r="C173" t="s">
+        <v>384</v>
+      </c>
+      <c r="D173" t="s">
         <v>385</v>
-      </c>
-      <c r="D173" t="s">
-        <v>386</v>
       </c>
       <c r="E173" s="3">
         <v>1979</v>
@@ -8318,10 +8707,10 @@
         <v>172</v>
       </c>
       <c r="C174" t="s">
+        <v>386</v>
+      </c>
+      <c r="D174" t="s">
         <v>387</v>
-      </c>
-      <c r="D174" t="s">
-        <v>388</v>
       </c>
       <c r="E174" s="3">
         <v>1967</v>
@@ -8358,10 +8747,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D00A50-BAF2-4D7C-9C79-39B14A850D5C}">
-  <dimension ref="B2:F175"/>
+  <dimension ref="B2:F176"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8374,19 +8763,19 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>392</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>490</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>393</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -8400,10 +8789,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -8417,10 +8806,10 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="5" spans="2:6">
@@ -8433,6 +8822,9 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
+      <c r="E5" t="s">
+        <v>534</v>
+      </c>
       <c r="F5" s="5"/>
     </row>
     <row r="6" spans="2:6">
@@ -8446,10 +8838,10 @@
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -8463,10 +8855,10 @@
         <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="8" spans="2:6">
@@ -8479,6 +8871,9 @@
       <c r="D8" t="s">
         <v>28</v>
       </c>
+      <c r="E8" t="s">
+        <v>535</v>
+      </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="2:6">
@@ -8491,6 +8886,9 @@
       <c r="D9" t="s">
         <v>31</v>
       </c>
+      <c r="E9" t="s">
+        <v>536</v>
+      </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:6">
@@ -8503,6 +8901,9 @@
       <c r="D10" t="s">
         <v>35</v>
       </c>
+      <c r="E10" t="s">
+        <v>537</v>
+      </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6">
@@ -8516,10 +8917,10 @@
         <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12" spans="2:6">
@@ -8532,6 +8933,9 @@
       <c r="D12" t="s">
         <v>42</v>
       </c>
+      <c r="E12" t="s">
+        <v>538</v>
+      </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6">
@@ -8544,6 +8948,9 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
+      <c r="E13" t="s">
+        <v>539</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6">
@@ -8557,10 +8964,10 @@
         <v>49</v>
       </c>
       <c r="E14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="15" spans="2:6">
@@ -8573,6 +8980,9 @@
       <c r="D15" t="s">
         <v>52</v>
       </c>
+      <c r="E15" t="s">
+        <v>540</v>
+      </c>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:6">
@@ -8585,6 +8995,9 @@
       <c r="D16" t="s">
         <v>54</v>
       </c>
+      <c r="E16" t="s">
+        <v>541</v>
+      </c>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="2:6">
@@ -8594,8 +9007,11 @@
       <c r="C17" s="9">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>56</v>
+      </c>
+      <c r="E17" t="s">
+        <v>542</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -8604,33 +9020,31 @@
         <v>16</v>
       </c>
       <c r="C18" s="9">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
-        <v>59</v>
+        <v>15</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>426</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>529</v>
-      </c>
+        <v>543</v>
+      </c>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="9">
         <v>17</v>
       </c>
       <c r="C19" s="9">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>499</v>
+        <v>528</v>
       </c>
     </row>
     <row r="20" spans="2:6">
@@ -8638,45 +9052,48 @@
         <v>18</v>
       </c>
       <c r="C20" s="9">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="E20" t="s">
+        <v>426</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="9">
         <v>19</v>
       </c>
       <c r="C21" s="9">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>400</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>501</v>
-      </c>
+        <v>544</v>
+      </c>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="9">
         <v>20</v>
       </c>
       <c r="C22" s="9">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" spans="2:6">
@@ -8684,51 +9101,62 @@
         <v>21</v>
       </c>
       <c r="C23" s="9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="E23" t="s">
+        <v>400</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="9">
         <v>22</v>
       </c>
       <c r="C24" s="9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>402</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>527</v>
-      </c>
+        <v>545</v>
+      </c>
+      <c r="F24" s="5"/>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" s="9">
         <v>23</v>
       </c>
       <c r="C25" s="9">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="E25" t="s">
+        <v>401</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="9">
         <v>24</v>
       </c>
       <c r="C26" s="9">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>546</v>
       </c>
       <c r="F26" s="5"/>
     </row>
@@ -8737,10 +9165,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="9">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>547</v>
       </c>
       <c r="F27" s="5"/>
     </row>
@@ -8749,62 +9180,63 @@
         <v>26</v>
       </c>
       <c r="C28" s="9">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>403</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>517</v>
-      </c>
+        <v>548</v>
+      </c>
+      <c r="F28" s="5"/>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="9">
         <v>27</v>
       </c>
       <c r="C29" s="9">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
-      </c>
-      <c r="F29" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="E29" t="s">
+        <v>402</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="9">
         <v>28</v>
       </c>
       <c r="C30" s="9">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E30" t="s">
-        <v>404</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>514</v>
-      </c>
+        <v>549</v>
+      </c>
+      <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="9">
         <v>29</v>
       </c>
       <c r="C31" s="9">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E31" t="s">
-        <v>428</v>
+        <v>403</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>491</v>
+        <v>513</v>
       </c>
     </row>
     <row r="32" spans="2:6">
@@ -8812,16 +9244,16 @@
         <v>30</v>
       </c>
       <c r="C32" s="9">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E32" t="s">
-        <v>405</v>
+        <v>427</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>526</v>
+        <v>490</v>
       </c>
     </row>
     <row r="33" spans="2:6">
@@ -8829,51 +9261,62 @@
         <v>31</v>
       </c>
       <c r="C33" s="9">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
-      </c>
-      <c r="F33" s="5"/>
+        <v>97</v>
+      </c>
+      <c r="E33" t="s">
+        <v>404</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="9">
         <v>32</v>
       </c>
       <c r="C34" s="9">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E34" t="s">
-        <v>406</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>511</v>
-      </c>
+        <v>550</v>
+      </c>
+      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="9">
         <v>33</v>
       </c>
       <c r="C35" s="9">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>103</v>
-      </c>
-      <c r="F35" s="5"/>
+        <v>101</v>
+      </c>
+      <c r="E35" t="s">
+        <v>405</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" s="9">
         <v>34</v>
       </c>
       <c r="C36" s="9">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>107</v>
+        <v>103</v>
+      </c>
+      <c r="E36" t="s">
+        <v>551</v>
       </c>
       <c r="F36" s="5"/>
     </row>
@@ -8882,10 +9325,13 @@
         <v>35</v>
       </c>
       <c r="C37" s="9">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="E37" t="s">
+        <v>552</v>
       </c>
       <c r="F37" s="5"/>
     </row>
@@ -8894,10 +9340,13 @@
         <v>36</v>
       </c>
       <c r="C38" s="9">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>109</v>
+      </c>
+      <c r="E38" t="s">
+        <v>553</v>
       </c>
       <c r="F38" s="5"/>
     </row>
@@ -8906,10 +9355,13 @@
         <v>37</v>
       </c>
       <c r="C39" s="9">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>114</v>
+        <v>112</v>
+      </c>
+      <c r="E39" t="s">
+        <v>554</v>
       </c>
       <c r="F39" s="5"/>
     </row>
@@ -8918,10 +9370,13 @@
         <v>38</v>
       </c>
       <c r="C40" s="9">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>119</v>
+        <v>114</v>
+      </c>
+      <c r="E40" t="s">
+        <v>555</v>
       </c>
       <c r="F40" s="5"/>
     </row>
@@ -8930,10 +9385,13 @@
         <v>39</v>
       </c>
       <c r="C41" s="9">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>121</v>
+        <v>119</v>
+      </c>
+      <c r="E41" t="s">
+        <v>556</v>
       </c>
       <c r="F41" s="5"/>
     </row>
@@ -8942,10 +9400,13 @@
         <v>40</v>
       </c>
       <c r="C42" s="9">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="E42" t="s">
+        <v>557</v>
       </c>
       <c r="F42" s="5"/>
     </row>
@@ -8954,39 +9415,45 @@
         <v>41</v>
       </c>
       <c r="C43" s="9">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
-        <v>407</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>516</v>
-      </c>
+        <v>558</v>
+      </c>
+      <c r="F43" s="5"/>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" s="9">
         <v>42</v>
       </c>
       <c r="C44" s="9">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D44" t="s">
-        <v>128</v>
-      </c>
-      <c r="F44" s="5"/>
+        <v>125</v>
+      </c>
+      <c r="E44" t="s">
+        <v>406</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="9">
         <v>43</v>
       </c>
       <c r="C45" s="9">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="E45" t="s">
+        <v>559</v>
       </c>
       <c r="F45" s="5"/>
     </row>
@@ -8995,10 +9462,13 @@
         <v>44</v>
       </c>
       <c r="C46" s="9">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>135</v>
+        <v>131</v>
+      </c>
+      <c r="E46" t="s">
+        <v>560</v>
       </c>
       <c r="F46" s="5"/>
     </row>
@@ -9007,10 +9477,13 @@
         <v>45</v>
       </c>
       <c r="C47" s="9">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="E47" t="s">
+        <v>561</v>
       </c>
       <c r="F47" s="5"/>
     </row>
@@ -9019,10 +9492,13 @@
         <v>46</v>
       </c>
       <c r="C48" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>138</v>
+        <v>136</v>
+      </c>
+      <c r="E48" t="s">
+        <v>562</v>
       </c>
       <c r="F48" s="5"/>
     </row>
@@ -9031,10 +9507,13 @@
         <v>47</v>
       </c>
       <c r="C49" s="9">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>139</v>
+        <v>138</v>
+      </c>
+      <c r="E49" t="s">
+        <v>563</v>
       </c>
       <c r="F49" s="5"/>
     </row>
@@ -9043,10 +9522,13 @@
         <v>48</v>
       </c>
       <c r="C50" s="9">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="E50" t="s">
+        <v>564</v>
       </c>
       <c r="F50" s="5"/>
     </row>
@@ -9055,39 +9537,45 @@
         <v>49</v>
       </c>
       <c r="C51" s="9">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E51" t="s">
-        <v>408</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>504</v>
-      </c>
+        <v>565</v>
+      </c>
+      <c r="F51" s="5"/>
     </row>
     <row r="52" spans="2:6">
       <c r="B52" s="9">
         <v>50</v>
       </c>
       <c r="C52" s="9">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>145</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>143</v>
+      </c>
+      <c r="E52" t="s">
+        <v>407</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53" s="9">
         <v>51</v>
       </c>
       <c r="C53" s="9">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="E53" t="s">
+        <v>566</v>
       </c>
       <c r="F53" s="5"/>
     </row>
@@ -9096,39 +9584,45 @@
         <v>52</v>
       </c>
       <c r="C54" s="9">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E54" t="s">
-        <v>429</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>521</v>
-      </c>
+        <v>567</v>
+      </c>
+      <c r="F54" s="5"/>
     </row>
     <row r="55" spans="2:6">
       <c r="B55" s="9">
         <v>53</v>
       </c>
       <c r="C55" s="9">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" t="s">
-        <v>155</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>152</v>
+      </c>
+      <c r="E55" t="s">
+        <v>428</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="56" spans="2:6">
       <c r="B56" s="9">
         <v>54</v>
       </c>
       <c r="C56" s="9">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D56" t="s">
-        <v>159</v>
+        <v>155</v>
+      </c>
+      <c r="E56" t="s">
+        <v>568</v>
       </c>
       <c r="F56" s="5"/>
     </row>
@@ -9137,10 +9631,13 @@
         <v>55</v>
       </c>
       <c r="C57" s="9">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" t="s">
-        <v>161</v>
+        <v>159</v>
+      </c>
+      <c r="E57" t="s">
+        <v>569</v>
       </c>
       <c r="F57" s="5"/>
     </row>
@@ -9149,10 +9646,13 @@
         <v>56</v>
       </c>
       <c r="C58" s="9">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+      <c r="E58" t="s">
+        <v>570</v>
       </c>
       <c r="F58" s="5"/>
     </row>
@@ -9161,10 +9661,13 @@
         <v>57</v>
       </c>
       <c r="C59" s="9">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D59" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="E59" t="s">
+        <v>571</v>
       </c>
       <c r="F59" s="5"/>
     </row>
@@ -9173,10 +9676,13 @@
         <v>58</v>
       </c>
       <c r="C60" s="9">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>167</v>
+        <v>165</v>
+      </c>
+      <c r="E60" t="s">
+        <v>572</v>
       </c>
       <c r="F60" s="5"/>
     </row>
@@ -9185,10 +9691,13 @@
         <v>59</v>
       </c>
       <c r="C61" s="9">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D61" t="s">
-        <v>170</v>
+        <v>167</v>
+      </c>
+      <c r="E61" t="s">
+        <v>573</v>
       </c>
       <c r="F61" s="5"/>
     </row>
@@ -9197,10 +9706,13 @@
         <v>60</v>
       </c>
       <c r="C62" s="9">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D62" t="s">
-        <v>172</v>
+        <v>170</v>
+      </c>
+      <c r="E62" t="s">
+        <v>574</v>
       </c>
       <c r="F62" s="5"/>
     </row>
@@ -9209,10 +9721,13 @@
         <v>61</v>
       </c>
       <c r="C63" s="9">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" t="s">
-        <v>175</v>
+        <v>172</v>
+      </c>
+      <c r="E63" t="s">
+        <v>575</v>
       </c>
       <c r="F63" s="5"/>
     </row>
@@ -9221,39 +9736,45 @@
         <v>62</v>
       </c>
       <c r="C64" s="9">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E64" t="s">
-        <v>409</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>532</v>
-      </c>
+        <v>576</v>
+      </c>
+      <c r="F64" s="5"/>
     </row>
     <row r="65" spans="2:6">
       <c r="B65" s="9">
         <v>63</v>
       </c>
       <c r="C65" s="9">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D65" t="s">
-        <v>178</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>176</v>
+      </c>
+      <c r="E65" t="s">
+        <v>408</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>531</v>
+      </c>
     </row>
     <row r="66" spans="2:6">
       <c r="B66" s="9">
         <v>64</v>
       </c>
       <c r="C66" s="9">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>180</v>
+        <v>178</v>
+      </c>
+      <c r="E66" t="s">
+        <v>577</v>
       </c>
       <c r="F66" s="5"/>
     </row>
@@ -9262,10 +9783,13 @@
         <v>65</v>
       </c>
       <c r="C67" s="9">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>183</v>
+        <v>180</v>
+      </c>
+      <c r="E67" t="s">
+        <v>578</v>
       </c>
       <c r="F67" s="5"/>
     </row>
@@ -9274,91 +9798,95 @@
         <v>66</v>
       </c>
       <c r="C68" s="9">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D68" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E68" t="s">
-        <v>410</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>500</v>
-      </c>
+        <v>579</v>
+      </c>
+      <c r="F68" s="5"/>
     </row>
     <row r="69" spans="2:6">
       <c r="B69" s="9">
         <v>67</v>
       </c>
       <c r="C69" s="9">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" t="s">
-        <v>187</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>185</v>
+      </c>
+      <c r="E69" t="s">
+        <v>409</v>
+      </c>
+      <c r="F69" s="5" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="70" spans="2:6">
       <c r="B70" s="9">
         <v>68</v>
       </c>
       <c r="C70" s="9">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D70" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E70" t="s">
-        <v>411</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>507</v>
-      </c>
+        <v>580</v>
+      </c>
+      <c r="F70" s="5"/>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" s="9">
         <v>69</v>
       </c>
       <c r="C71" s="9">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D71" t="s">
-        <v>191</v>
-      </c>
-      <c r="F71" s="5"/>
+        <v>189</v>
+      </c>
+      <c r="E71" t="s">
+        <v>410</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" s="9">
         <v>70</v>
       </c>
       <c r="C72" s="9">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D72" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E72" t="s">
-        <v>412</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>531</v>
-      </c>
+        <v>581</v>
+      </c>
+      <c r="F72" s="5"/>
     </row>
     <row r="73" spans="2:6">
       <c r="B73" s="9">
         <v>71</v>
       </c>
       <c r="C73" s="9">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D73" t="s">
-        <v>196</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>413</v>
+        <v>193</v>
+      </c>
+      <c r="E73" t="s">
+        <v>411</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>506</v>
+        <v>530</v>
       </c>
     </row>
     <row r="74" spans="2:6">
@@ -9366,22 +9894,30 @@
         <v>72</v>
       </c>
       <c r="C74" s="9">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D74" t="s">
-        <v>199</v>
-      </c>
-      <c r="F74" s="5"/>
+        <v>196</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="75" spans="2:6">
       <c r="B75" s="9">
         <v>73</v>
       </c>
       <c r="C75" s="9">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D75" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="E75" t="s">
+        <v>582</v>
       </c>
       <c r="F75" s="5"/>
     </row>
@@ -9390,39 +9926,45 @@
         <v>74</v>
       </c>
       <c r="C76" s="9">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D76" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E76" t="s">
-        <v>430</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>528</v>
-      </c>
+        <v>583</v>
+      </c>
+      <c r="F76" s="5"/>
     </row>
     <row r="77" spans="2:6">
       <c r="B77" s="9">
         <v>75</v>
       </c>
       <c r="C77" s="9">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D77" t="s">
-        <v>205</v>
-      </c>
-      <c r="F77" s="5"/>
+        <v>203</v>
+      </c>
+      <c r="E77" t="s">
+        <v>429</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>527</v>
+      </c>
     </row>
     <row r="78" spans="2:6">
       <c r="B78" s="9">
         <v>76</v>
       </c>
       <c r="C78" s="9">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D78" t="s">
-        <v>207</v>
+        <v>205</v>
+      </c>
+      <c r="E78" t="s">
+        <v>584</v>
       </c>
       <c r="F78" s="5"/>
     </row>
@@ -9431,62 +9973,63 @@
         <v>77</v>
       </c>
       <c r="C79" s="9">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D79" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E79" t="s">
-        <v>431</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>533</v>
-      </c>
+        <v>585</v>
+      </c>
+      <c r="F79" s="5"/>
     </row>
     <row r="80" spans="2:6">
       <c r="B80" s="9">
         <v>78</v>
       </c>
       <c r="C80" s="9">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D80" t="s">
-        <v>211</v>
-      </c>
-      <c r="F80" s="5"/>
+        <v>208</v>
+      </c>
+      <c r="E80" t="s">
+        <v>430</v>
+      </c>
+      <c r="F80" s="5" t="s">
+        <v>532</v>
+      </c>
     </row>
     <row r="81" spans="2:6">
       <c r="B81" s="9">
         <v>79</v>
       </c>
       <c r="C81" s="9">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D81" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E81" t="s">
-        <v>414</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>492</v>
-      </c>
+        <v>586</v>
+      </c>
+      <c r="F81" s="5"/>
     </row>
     <row r="82" spans="2:6">
       <c r="B82" s="9">
         <v>80</v>
       </c>
       <c r="C82" s="9">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D82" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E82" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
     </row>
     <row r="83" spans="2:6">
@@ -9494,80 +10037,94 @@
         <v>81</v>
       </c>
       <c r="C83" s="9">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D83" t="s">
-        <v>216</v>
-      </c>
-      <c r="F83" s="5"/>
+        <v>215</v>
+      </c>
+      <c r="E83" t="s">
+        <v>431</v>
+      </c>
+      <c r="F83" s="5" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="84" spans="2:6">
       <c r="B84" s="9">
         <v>82</v>
       </c>
       <c r="C84" s="9">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D84" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E84" t="s">
-        <v>415</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>513</v>
-      </c>
+        <v>587</v>
+      </c>
+      <c r="F84" s="5"/>
     </row>
     <row r="85" spans="2:6">
       <c r="B85" s="9">
         <v>83</v>
       </c>
       <c r="C85" s="9">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D85" t="s">
-        <v>222</v>
-      </c>
-      <c r="F85" s="5"/>
+        <v>218</v>
+      </c>
+      <c r="E85" t="s">
+        <v>414</v>
+      </c>
+      <c r="F85" s="5" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="86" spans="2:6">
       <c r="B86" s="9">
         <v>84</v>
       </c>
       <c r="C86" s="9">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D86" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E86" t="s">
-        <v>416</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>518</v>
-      </c>
+        <v>588</v>
+      </c>
+      <c r="F86" s="5"/>
     </row>
     <row r="87" spans="2:6">
       <c r="B87" s="9">
         <v>85</v>
       </c>
       <c r="C87" s="9">
-        <v>85</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="F87" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="D87" t="s">
+        <v>224</v>
+      </c>
+      <c r="E87" t="s">
+        <v>415</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="88" spans="2:6">
       <c r="B88" s="9">
         <v>86</v>
       </c>
       <c r="C88" s="9">
-        <v>86</v>
-      </c>
-      <c r="D88" t="s">
-        <v>229</v>
+        <v>85</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E88" t="s">
+        <v>589</v>
       </c>
       <c r="F88" s="5"/>
     </row>
@@ -9576,39 +10133,45 @@
         <v>87</v>
       </c>
       <c r="C89" s="9">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D89" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E89" t="s">
-        <v>417</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>515</v>
-      </c>
+        <v>590</v>
+      </c>
+      <c r="F89" s="5"/>
     </row>
     <row r="90" spans="2:6">
       <c r="B90" s="9">
         <v>88</v>
       </c>
       <c r="C90" s="9">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D90" t="s">
-        <v>233</v>
-      </c>
-      <c r="F90" s="5"/>
+        <v>231</v>
+      </c>
+      <c r="E90" t="s">
+        <v>416</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="91" spans="2:6">
       <c r="B91" s="9">
         <v>89</v>
       </c>
       <c r="C91" s="9">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D91" t="s">
-        <v>235</v>
+        <v>233</v>
+      </c>
+      <c r="E91" t="s">
+        <v>591</v>
       </c>
       <c r="F91" s="5"/>
     </row>
@@ -9617,10 +10180,13 @@
         <v>90</v>
       </c>
       <c r="C92" s="9">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D92" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="E92" t="s">
+        <v>592</v>
       </c>
       <c r="F92" s="5"/>
     </row>
@@ -9629,10 +10195,13 @@
         <v>91</v>
       </c>
       <c r="C93" s="9">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D93" t="s">
-        <v>240</v>
+        <v>237</v>
+      </c>
+      <c r="E93" t="s">
+        <v>593</v>
       </c>
       <c r="F93" s="5"/>
     </row>
@@ -9641,39 +10210,45 @@
         <v>92</v>
       </c>
       <c r="C94" s="9">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D94" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E94" t="s">
-        <v>418</v>
-      </c>
-      <c r="F94" s="5" t="s">
-        <v>495</v>
-      </c>
+        <v>594</v>
+      </c>
+      <c r="F94" s="5"/>
     </row>
     <row r="95" spans="2:6">
       <c r="B95" s="9">
         <v>93</v>
       </c>
       <c r="C95" s="9">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D95" t="s">
-        <v>246</v>
-      </c>
-      <c r="F95" s="5"/>
+        <v>243</v>
+      </c>
+      <c r="E95" t="s">
+        <v>417</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="96" spans="2:6">
       <c r="B96" s="9">
         <v>94</v>
       </c>
       <c r="C96" s="9">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D96" t="s">
-        <v>248</v>
+        <v>246</v>
+      </c>
+      <c r="E96" t="s">
+        <v>595</v>
       </c>
       <c r="F96" s="5"/>
     </row>
@@ -9682,10 +10257,13 @@
         <v>95</v>
       </c>
       <c r="C97" s="9">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D97" t="s">
-        <v>250</v>
+        <v>248</v>
+      </c>
+      <c r="E97" t="s">
+        <v>596</v>
       </c>
       <c r="F97" s="5"/>
     </row>
@@ -9694,10 +10272,13 @@
         <v>96</v>
       </c>
       <c r="C98" s="9">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D98" t="s">
-        <v>253</v>
+        <v>250</v>
+      </c>
+      <c r="E98" t="s">
+        <v>597</v>
       </c>
       <c r="F98" s="5"/>
     </row>
@@ -9706,10 +10287,13 @@
         <v>97</v>
       </c>
       <c r="C99" s="9">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D99" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="E99" t="s">
+        <v>598</v>
       </c>
       <c r="F99" s="5"/>
     </row>
@@ -9718,10 +10302,13 @@
         <v>98</v>
       </c>
       <c r="C100" s="9">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D100" t="s">
-        <v>257</v>
+        <v>255</v>
+      </c>
+      <c r="E100" t="s">
+        <v>599</v>
       </c>
       <c r="F100" s="5"/>
     </row>
@@ -9730,10 +10317,13 @@
         <v>99</v>
       </c>
       <c r="C101" s="9">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D101" t="s">
-        <v>259</v>
+        <v>257</v>
+      </c>
+      <c r="E101" t="s">
+        <v>600</v>
       </c>
       <c r="F101" s="5"/>
     </row>
@@ -9742,10 +10332,13 @@
         <v>100</v>
       </c>
       <c r="C102" s="9">
-        <v>100</v>
-      </c>
-      <c r="D102" s="8" t="s">
-        <v>260</v>
+        <v>99</v>
+      </c>
+      <c r="D102" t="s">
+        <v>259</v>
+      </c>
+      <c r="E102" t="s">
+        <v>601</v>
       </c>
       <c r="F102" s="5"/>
     </row>
@@ -9754,10 +10347,13 @@
         <v>101</v>
       </c>
       <c r="C103" s="9">
-        <v>101</v>
-      </c>
-      <c r="D103" t="s">
-        <v>262</v>
+        <v>100</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E103" t="s">
+        <v>602</v>
       </c>
       <c r="F103" s="5"/>
     </row>
@@ -9766,10 +10362,13 @@
         <v>102</v>
       </c>
       <c r="C104" s="9">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D104" t="s">
-        <v>264</v>
+        <v>262</v>
+      </c>
+      <c r="E104" t="s">
+        <v>603</v>
       </c>
       <c r="F104" s="5"/>
     </row>
@@ -9778,10 +10377,13 @@
         <v>103</v>
       </c>
       <c r="C105" s="9">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D105" t="s">
-        <v>265</v>
+        <v>264</v>
+      </c>
+      <c r="E105" t="s">
+        <v>604</v>
       </c>
       <c r="F105" s="5"/>
     </row>
@@ -9790,39 +10392,39 @@
         <v>104</v>
       </c>
       <c r="C106" s="9">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D106" t="s">
-        <v>267</v>
-      </c>
-      <c r="E106" t="s">
-        <v>433</v>
-      </c>
-      <c r="F106" s="5" t="s">
-        <v>530</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="F106" s="5"/>
     </row>
     <row r="107" spans="2:6">
       <c r="B107" s="9">
         <v>105</v>
       </c>
       <c r="C107" s="9">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D107" t="s">
-        <v>269</v>
-      </c>
-      <c r="F107" s="5"/>
+        <v>267</v>
+      </c>
+      <c r="E107" t="s">
+        <v>432</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>529</v>
+      </c>
     </row>
     <row r="108" spans="2:6">
       <c r="B108" s="9">
         <v>106</v>
       </c>
       <c r="C108" s="9">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D108" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F108" s="5"/>
     </row>
@@ -9831,10 +10433,13 @@
         <v>107</v>
       </c>
       <c r="C109" s="9">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D109" t="s">
-        <v>273</v>
+        <v>271</v>
+      </c>
+      <c r="E109" t="s">
+        <v>605</v>
       </c>
       <c r="F109" s="5"/>
     </row>
@@ -9843,10 +10448,13 @@
         <v>108</v>
       </c>
       <c r="C110" s="9">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D110" t="s">
-        <v>274</v>
+        <v>273</v>
+      </c>
+      <c r="E110" t="s">
+        <v>606</v>
       </c>
       <c r="F110" s="5"/>
     </row>
@@ -9855,10 +10463,13 @@
         <v>109</v>
       </c>
       <c r="C111" s="9">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D111" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+      <c r="E111" t="s">
+        <v>607</v>
       </c>
       <c r="F111" s="5"/>
     </row>
@@ -9867,10 +10478,13 @@
         <v>110</v>
       </c>
       <c r="C112" s="9">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D112" t="s">
-        <v>276</v>
+        <v>275</v>
+      </c>
+      <c r="E112" t="s">
+        <v>608</v>
       </c>
       <c r="F112" s="5"/>
     </row>
@@ -9879,10 +10493,13 @@
         <v>111</v>
       </c>
       <c r="C113" s="9">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D113" t="s">
-        <v>277</v>
+        <v>276</v>
+      </c>
+      <c r="E113" t="s">
+        <v>609</v>
       </c>
       <c r="F113" s="5"/>
     </row>
@@ -9891,10 +10508,13 @@
         <v>112</v>
       </c>
       <c r="C114" s="9">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D114" t="s">
-        <v>279</v>
+        <v>277</v>
+      </c>
+      <c r="E114" t="s">
+        <v>610</v>
       </c>
       <c r="F114" s="5"/>
     </row>
@@ -9903,10 +10523,13 @@
         <v>113</v>
       </c>
       <c r="C115" s="9">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D115" t="s">
-        <v>282</v>
+        <v>279</v>
+      </c>
+      <c r="E115" t="s">
+        <v>611</v>
       </c>
       <c r="F115" s="5"/>
     </row>
@@ -9915,39 +10538,45 @@
         <v>114</v>
       </c>
       <c r="C116" s="9">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D116" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E116" t="s">
-        <v>419</v>
-      </c>
-      <c r="F116" s="5" t="s">
-        <v>503</v>
-      </c>
+        <v>612</v>
+      </c>
+      <c r="F116" s="5"/>
     </row>
     <row r="117" spans="2:6">
       <c r="B117" s="9">
         <v>115</v>
       </c>
       <c r="C117" s="9">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D117" t="s">
-        <v>286</v>
-      </c>
-      <c r="F117" s="5"/>
+        <v>284</v>
+      </c>
+      <c r="E117" t="s">
+        <v>418</v>
+      </c>
+      <c r="F117" s="5" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="118" spans="2:6">
       <c r="B118" s="9">
         <v>116</v>
       </c>
       <c r="C118" s="9">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D118" t="s">
-        <v>287</v>
+        <v>286</v>
+      </c>
+      <c r="E118" t="s">
+        <v>613</v>
       </c>
       <c r="F118" s="5"/>
     </row>
@@ -9956,10 +10585,13 @@
         <v>117</v>
       </c>
       <c r="C119" s="9">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D119" t="s">
-        <v>289</v>
+        <v>287</v>
+      </c>
+      <c r="E119" t="s">
+        <v>614</v>
       </c>
       <c r="F119" s="5"/>
     </row>
@@ -9968,10 +10600,13 @@
         <v>118</v>
       </c>
       <c r="C120" s="9">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D120" t="s">
-        <v>291</v>
+        <v>289</v>
+      </c>
+      <c r="E120" t="s">
+        <v>615</v>
       </c>
       <c r="F120" s="5"/>
     </row>
@@ -9980,10 +10615,13 @@
         <v>119</v>
       </c>
       <c r="C121" s="9">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D121" t="s">
-        <v>293</v>
+        <v>291</v>
+      </c>
+      <c r="E121" t="s">
+        <v>616</v>
       </c>
       <c r="F121" s="5"/>
     </row>
@@ -9992,10 +10630,13 @@
         <v>120</v>
       </c>
       <c r="C122" s="9">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D122" t="s">
-        <v>294</v>
+        <v>293</v>
+      </c>
+      <c r="E122" t="s">
+        <v>617</v>
       </c>
       <c r="F122" s="5"/>
     </row>
@@ -10004,10 +10645,13 @@
         <v>121</v>
       </c>
       <c r="C123" s="9">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D123" t="s">
-        <v>295</v>
+        <v>294</v>
+      </c>
+      <c r="E123" t="s">
+        <v>618</v>
       </c>
       <c r="F123" s="5"/>
     </row>
@@ -10016,10 +10660,13 @@
         <v>122</v>
       </c>
       <c r="C124" s="9">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D124" t="s">
-        <v>299</v>
+        <v>295</v>
+      </c>
+      <c r="E124" t="s">
+        <v>619</v>
       </c>
       <c r="F124" s="5"/>
     </row>
@@ -10028,39 +10675,45 @@
         <v>123</v>
       </c>
       <c r="C125" s="9">
-        <v>123</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>301</v>
+        <v>122</v>
+      </c>
+      <c r="D125" t="s">
+        <v>299</v>
       </c>
       <c r="E125" t="s">
-        <v>434</v>
-      </c>
-      <c r="F125" s="5" t="s">
-        <v>523</v>
-      </c>
+        <v>620</v>
+      </c>
+      <c r="F125" s="5"/>
     </row>
     <row r="126" spans="2:6">
       <c r="B126" s="9">
         <v>124</v>
       </c>
       <c r="C126" s="9">
-        <v>124</v>
-      </c>
-      <c r="D126" t="s">
-        <v>303</v>
-      </c>
-      <c r="F126" s="5"/>
+        <v>123</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E126" t="s">
+        <v>433</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="127" spans="2:6">
       <c r="B127" s="9">
         <v>125</v>
       </c>
       <c r="C127" s="9">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D127" t="s">
-        <v>305</v>
+        <v>303</v>
+      </c>
+      <c r="E127" t="s">
+        <v>621</v>
       </c>
       <c r="F127" s="5"/>
     </row>
@@ -10069,10 +10722,13 @@
         <v>126</v>
       </c>
       <c r="C128" s="9">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D128" t="s">
-        <v>308</v>
+        <v>305</v>
+      </c>
+      <c r="E128" t="s">
+        <v>622</v>
       </c>
       <c r="F128" s="5"/>
     </row>
@@ -10081,10 +10737,13 @@
         <v>127</v>
       </c>
       <c r="C129" s="9">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D129" t="s">
-        <v>310</v>
+        <v>308</v>
+      </c>
+      <c r="E129" t="s">
+        <v>623</v>
       </c>
       <c r="F129" s="5"/>
     </row>
@@ -10093,10 +10752,13 @@
         <v>128</v>
       </c>
       <c r="C130" s="9">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D130" t="s">
-        <v>312</v>
+        <v>310</v>
+      </c>
+      <c r="E130" t="s">
+        <v>624</v>
       </c>
       <c r="F130" s="5"/>
     </row>
@@ -10105,10 +10767,13 @@
         <v>129</v>
       </c>
       <c r="C131" s="9">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D131" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="E131" t="s">
+        <v>625</v>
       </c>
       <c r="F131" s="5"/>
     </row>
@@ -10117,10 +10782,13 @@
         <v>130</v>
       </c>
       <c r="C132" s="9">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D132" t="s">
-        <v>314</v>
+        <v>313</v>
+      </c>
+      <c r="E132" t="s">
+        <v>626</v>
       </c>
       <c r="F132" s="5"/>
     </row>
@@ -10129,39 +10797,45 @@
         <v>131</v>
       </c>
       <c r="C133" s="9">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D133" t="s">
-        <v>316</v>
+        <v>627</v>
       </c>
       <c r="E133" t="s">
-        <v>420</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>509</v>
-      </c>
+        <v>628</v>
+      </c>
+      <c r="F133" s="5"/>
     </row>
     <row r="134" spans="2:6">
       <c r="B134" s="9">
         <v>132</v>
       </c>
       <c r="C134" s="9">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D134" t="s">
-        <v>317</v>
-      </c>
-      <c r="F134" s="5"/>
+        <v>315</v>
+      </c>
+      <c r="E134" t="s">
+        <v>419</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="135" spans="2:6">
       <c r="B135" s="9">
         <v>133</v>
       </c>
       <c r="C135" s="9">
-        <v>133</v>
-      </c>
-      <c r="D135" s="4" t="s">
-        <v>319</v>
+        <v>132</v>
+      </c>
+      <c r="D135" t="s">
+        <v>316</v>
+      </c>
+      <c r="E135" t="s">
+        <v>629</v>
       </c>
       <c r="F135" s="5"/>
     </row>
@@ -10170,10 +10844,10 @@
         <v>134</v>
       </c>
       <c r="C136" s="9">
-        <v>134</v>
-      </c>
-      <c r="D136" t="s">
-        <v>321</v>
+        <v>133</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>318</v>
       </c>
       <c r="F136" s="5"/>
     </row>
@@ -10182,10 +10856,13 @@
         <v>135</v>
       </c>
       <c r="C137" s="9">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D137" t="s">
-        <v>322</v>
+        <v>320</v>
+      </c>
+      <c r="E137" t="s">
+        <v>630</v>
       </c>
       <c r="F137" s="5"/>
     </row>
@@ -10194,10 +10871,13 @@
         <v>136</v>
       </c>
       <c r="C138" s="9">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D138" t="s">
-        <v>324</v>
+        <v>321</v>
+      </c>
+      <c r="E138" t="s">
+        <v>631</v>
       </c>
       <c r="F138" s="5"/>
     </row>
@@ -10206,10 +10886,13 @@
         <v>137</v>
       </c>
       <c r="C139" s="9">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D139" t="s">
-        <v>325</v>
+        <v>323</v>
+      </c>
+      <c r="E139" t="s">
+        <v>632</v>
       </c>
       <c r="F139" s="5"/>
     </row>
@@ -10218,10 +10901,13 @@
         <v>138</v>
       </c>
       <c r="C140" s="9">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D140" t="s">
-        <v>326</v>
+        <v>324</v>
+      </c>
+      <c r="E140" t="s">
+        <v>633</v>
       </c>
       <c r="F140" s="5"/>
     </row>
@@ -10230,10 +10916,13 @@
         <v>139</v>
       </c>
       <c r="C141" s="9">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D141" t="s">
-        <v>330</v>
+        <v>325</v>
+      </c>
+      <c r="E141" t="s">
+        <v>634</v>
       </c>
       <c r="F141" s="5"/>
     </row>
@@ -10242,10 +10931,13 @@
         <v>140</v>
       </c>
       <c r="C142" s="9">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D142" t="s">
-        <v>332</v>
+        <v>329</v>
+      </c>
+      <c r="E142" t="s">
+        <v>635</v>
       </c>
       <c r="F142" s="5"/>
     </row>
@@ -10254,10 +10946,13 @@
         <v>141</v>
       </c>
       <c r="C143" s="9">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D143" t="s">
-        <v>334</v>
+        <v>331</v>
+      </c>
+      <c r="E143" t="s">
+        <v>636</v>
       </c>
       <c r="F143" s="5"/>
     </row>
@@ -10266,33 +10961,28 @@
         <v>142</v>
       </c>
       <c r="C144" s="9">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D144" t="s">
-        <v>336</v>
-      </c>
-      <c r="E144" t="s">
-        <v>435</v>
-      </c>
-      <c r="F144" s="5" t="s">
-        <v>510</v>
-      </c>
+        <v>333</v>
+      </c>
+      <c r="F144" s="5"/>
     </row>
     <row r="145" spans="2:6">
       <c r="B145" s="9">
         <v>143</v>
       </c>
       <c r="C145" s="9">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D145" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E145" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F145" s="5" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
     </row>
     <row r="146" spans="2:6">
@@ -10300,22 +10990,30 @@
         <v>144</v>
       </c>
       <c r="C146" s="9">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D146" t="s">
-        <v>340</v>
-      </c>
-      <c r="F146" s="5"/>
+        <v>337</v>
+      </c>
+      <c r="E146" t="s">
+        <v>435</v>
+      </c>
+      <c r="F146" s="5" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="147" spans="2:6">
       <c r="B147" s="9">
         <v>145</v>
       </c>
       <c r="C147" s="9">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D147" t="s">
-        <v>343</v>
+        <v>339</v>
+      </c>
+      <c r="E147" t="s">
+        <v>637</v>
       </c>
       <c r="F147" s="5"/>
     </row>
@@ -10324,10 +11022,13 @@
         <v>146</v>
       </c>
       <c r="C148" s="9">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D148" t="s">
-        <v>345</v>
+        <v>342</v>
+      </c>
+      <c r="E148" t="s">
+        <v>638</v>
       </c>
       <c r="F148" s="5"/>
     </row>
@@ -10336,10 +11037,13 @@
         <v>147</v>
       </c>
       <c r="C149" s="9">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D149" t="s">
-        <v>346</v>
+        <v>344</v>
+      </c>
+      <c r="E149" t="s">
+        <v>639</v>
       </c>
       <c r="F149" s="5"/>
     </row>
@@ -10348,10 +11052,13 @@
         <v>148</v>
       </c>
       <c r="C150" s="9">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D150" t="s">
-        <v>348</v>
+        <v>345</v>
+      </c>
+      <c r="E150" t="s">
+        <v>640</v>
       </c>
       <c r="F150" s="5"/>
     </row>
@@ -10360,10 +11067,13 @@
         <v>149</v>
       </c>
       <c r="C151" s="9">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D151" t="s">
-        <v>349</v>
+        <v>347</v>
+      </c>
+      <c r="E151" t="s">
+        <v>641</v>
       </c>
       <c r="F151" s="5"/>
     </row>
@@ -10372,33 +11082,31 @@
         <v>150</v>
       </c>
       <c r="C152" s="9">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D152" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E152" t="s">
-        <v>437</v>
-      </c>
-      <c r="F152" s="5" t="s">
-        <v>508</v>
-      </c>
+        <v>642</v>
+      </c>
+      <c r="F152" s="5"/>
     </row>
     <row r="153" spans="2:6">
       <c r="B153" s="9">
         <v>151</v>
       </c>
       <c r="C153" s="9">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D153" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E153" t="s">
-        <v>421</v>
+        <v>436</v>
       </c>
       <c r="F153" s="5" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
     </row>
     <row r="154" spans="2:6">
@@ -10406,16 +11114,16 @@
         <v>152</v>
       </c>
       <c r="C154" s="9">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D154" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E154" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F154" s="5" t="s">
-        <v>505</v>
+        <v>523</v>
       </c>
     </row>
     <row r="155" spans="2:6">
@@ -10423,16 +11131,16 @@
         <v>153</v>
       </c>
       <c r="C155" s="9">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D155" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E155" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F155" s="5" t="s">
-        <v>519</v>
+        <v>504</v>
       </c>
     </row>
     <row r="156" spans="2:6">
@@ -10440,51 +11148,62 @@
         <v>154</v>
       </c>
       <c r="C156" s="9">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D156" t="s">
-        <v>355</v>
-      </c>
-      <c r="F156" s="5"/>
+        <v>352</v>
+      </c>
+      <c r="E156" t="s">
+        <v>422</v>
+      </c>
+      <c r="F156" s="5" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="157" spans="2:6">
       <c r="B157" s="9">
         <v>155</v>
       </c>
       <c r="C157" s="9">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D157" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="E157" t="s">
-        <v>438</v>
-      </c>
-      <c r="F157" s="5" t="s">
-        <v>497</v>
-      </c>
+        <v>643</v>
+      </c>
+      <c r="F157" s="5"/>
     </row>
     <row r="158" spans="2:6">
       <c r="B158" s="9">
         <v>156</v>
       </c>
       <c r="C158" s="9">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D158" t="s">
-        <v>359</v>
-      </c>
-      <c r="F158" s="5"/>
+        <v>356</v>
+      </c>
+      <c r="E158" t="s">
+        <v>437</v>
+      </c>
+      <c r="F158" s="5" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="159" spans="2:6">
       <c r="B159" s="9">
         <v>157</v>
       </c>
       <c r="C159" s="9">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D159" t="s">
-        <v>360</v>
+        <v>358</v>
+      </c>
+      <c r="E159" t="s">
+        <v>644</v>
       </c>
       <c r="F159" s="5"/>
     </row>
@@ -10493,10 +11212,13 @@
         <v>158</v>
       </c>
       <c r="C160" s="9">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D160" t="s">
-        <v>362</v>
+        <v>359</v>
+      </c>
+      <c r="E160" t="s">
+        <v>645</v>
       </c>
       <c r="F160" s="5"/>
     </row>
@@ -10505,10 +11227,13 @@
         <v>159</v>
       </c>
       <c r="C161" s="9">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D161" t="s">
-        <v>364</v>
+        <v>361</v>
+      </c>
+      <c r="E161" t="s">
+        <v>646</v>
       </c>
       <c r="F161" s="5"/>
     </row>
@@ -10517,10 +11242,13 @@
         <v>160</v>
       </c>
       <c r="C162" s="9">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D162" t="s">
-        <v>366</v>
+        <v>363</v>
+      </c>
+      <c r="E162" t="s">
+        <v>647</v>
       </c>
       <c r="F162" s="5"/>
     </row>
@@ -10529,10 +11257,10 @@
         <v>161</v>
       </c>
       <c r="C163" s="9">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D163" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F163" s="5"/>
     </row>
@@ -10541,10 +11269,13 @@
         <v>162</v>
       </c>
       <c r="C164" s="9">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D164" t="s">
-        <v>369</v>
+        <v>366</v>
+      </c>
+      <c r="E164" t="s">
+        <v>648</v>
       </c>
       <c r="F164" s="5"/>
     </row>
@@ -10553,10 +11284,13 @@
         <v>163</v>
       </c>
       <c r="C165" s="9">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D165" t="s">
-        <v>371</v>
+        <v>368</v>
+      </c>
+      <c r="E165" t="s">
+        <v>649</v>
       </c>
       <c r="F165" s="5"/>
     </row>
@@ -10565,10 +11299,13 @@
         <v>164</v>
       </c>
       <c r="C166" s="9">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D166" t="s">
-        <v>372</v>
+        <v>370</v>
+      </c>
+      <c r="E166" t="s">
+        <v>650</v>
       </c>
       <c r="F166" s="5"/>
     </row>
@@ -10577,10 +11314,13 @@
         <v>165</v>
       </c>
       <c r="C167" s="9">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D167" t="s">
-        <v>374</v>
+        <v>371</v>
+      </c>
+      <c r="E167" t="s">
+        <v>651</v>
       </c>
       <c r="F167" s="5"/>
     </row>
@@ -10589,10 +11329,13 @@
         <v>166</v>
       </c>
       <c r="C168" s="9">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D168" t="s">
-        <v>376</v>
+        <v>373</v>
+      </c>
+      <c r="E168" t="s">
+        <v>652</v>
       </c>
       <c r="F168" s="5"/>
     </row>
@@ -10601,10 +11344,13 @@
         <v>167</v>
       </c>
       <c r="C169" s="9">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D169" t="s">
-        <v>378</v>
+        <v>375</v>
+      </c>
+      <c r="E169" t="s">
+        <v>653</v>
       </c>
       <c r="F169" s="5"/>
     </row>
@@ -10613,10 +11359,13 @@
         <v>168</v>
       </c>
       <c r="C170" s="9">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D170" t="s">
-        <v>379</v>
+        <v>377</v>
+      </c>
+      <c r="E170" t="s">
+        <v>654</v>
       </c>
       <c r="F170" s="5"/>
     </row>
@@ -10625,10 +11374,13 @@
         <v>169</v>
       </c>
       <c r="C171" s="9">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D171" t="s">
-        <v>381</v>
+        <v>378</v>
+      </c>
+      <c r="E171" t="s">
+        <v>655</v>
       </c>
       <c r="F171" s="5"/>
     </row>
@@ -10637,10 +11389,13 @@
         <v>170</v>
       </c>
       <c r="C172" s="9">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D172" t="s">
-        <v>384</v>
+        <v>380</v>
+      </c>
+      <c r="E172" t="s">
+        <v>656</v>
       </c>
       <c r="F172" s="5"/>
     </row>
@@ -10649,10 +11404,10 @@
         <v>171</v>
       </c>
       <c r="C173" s="9">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D173" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F173" s="5"/>
     </row>
@@ -10661,41 +11416,59 @@
         <v>172</v>
       </c>
       <c r="C174" s="9">
+        <v>171</v>
+      </c>
+      <c r="D174" t="s">
+        <v>384</v>
+      </c>
+      <c r="E174" t="s">
+        <v>657</v>
+      </c>
+      <c r="F174" s="5"/>
+    </row>
+    <row r="175" spans="2:6">
+      <c r="B175" s="9">
+        <v>173</v>
+      </c>
+      <c r="C175" s="9">
         <v>172</v>
       </c>
-      <c r="D174" t="s">
-        <v>387</v>
-      </c>
-      <c r="E174" t="s">
+      <c r="D175" t="s">
+        <v>386</v>
+      </c>
+      <c r="E175" t="s">
+        <v>438</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="176" spans="2:6">
+      <c r="B176" t="s">
         <v>439</v>
       </c>
-      <c r="F174" s="5" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="175" spans="2:6">
-      <c r="B175" t="s">
-        <v>440</v>
-      </c>
-      <c r="E175">
+      <c r="E176">
         <f>SUBTOTAL(103,Tabela2[File Name])</f>
-        <v>44</v>
-      </c>
-      <c r="F175">
+        <v>167</v>
+      </c>
+      <c r="F176">
         <f>SUBTOTAL(103,Tabela2[File Adress])</f>
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E3:E174">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="E3:E4 E6:E12 E14 E16:E48 E50:E103 E105:E132 E134:E175">
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F174">
+  <conditionalFormatting sqref="F3:F175">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E175">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F31" r:id="rId1" xr:uid="{68B4E8A5-0080-4372-B4E0-62930C0A68B4}"/>
-    <hyperlink ref="F28" r:id="rId2" xr:uid="{AD28D80B-ECEE-4289-A1F7-69B4666DA64D}"/>
+    <hyperlink ref="F32" r:id="rId1" xr:uid="{68B4E8A5-0080-4372-B4E0-62930C0A68B4}"/>
+    <hyperlink ref="F29" r:id="rId2" xr:uid="{AD28D80B-ECEE-4289-A1F7-69B4666DA64D}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">

</xml_diff>